<commit_message>
Scaffold de algunas páginas.
</commit_message>
<xml_diff>
--- a/Proyecto - Entrega Final/IgnisMercado/- - Documentos/migracion.xlsx
+++ b/Proyecto - Entrega Final/IgnisMercado/- - Documentos/migracion.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PII-Proyecto-2019-Marcelo\IgnisMercado\- - Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABBDD21-0079-4E6E-A634-B79CA9A18607}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43AF440-CE68-4DF9-8B1D-881C279C120A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{54F86B65-C9D8-49FD-B121-67B152A46407}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{54F86B65-C9D8-49FD-B121-67B152A46407}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="86">
   <si>
     <t>e75bccb1-9c96-4ae1-86a4-6230c0f1e880</t>
   </si>
@@ -285,6 +286,9 @@
   </si>
   <si>
     <t>58a7e2bd-ed5f-4867-89b6-2b834b8ca1fe</t>
+  </si>
+  <si>
+    <t>SolicitudId</t>
   </si>
 </sst>
 </file>
@@ -484,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -551,6 +555,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -866,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A2DB2C-95A7-493E-8353-D6063C63B1B1}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,6 +1143,7 @@
       <c r="E15" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
@@ -1153,6 +1161,7 @@
       <c r="E16" s="16">
         <v>1</v>
       </c>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
@@ -1170,6 +1179,7 @@
       <c r="E17" s="16">
         <v>1</v>
       </c>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
@@ -1187,6 +1197,7 @@
       <c r="E18" s="16">
         <v>1</v>
       </c>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
@@ -1204,6 +1215,7 @@
       <c r="E19" s="16">
         <v>1</v>
       </c>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
@@ -1221,6 +1233,7 @@
       <c r="E20" s="16">
         <v>1</v>
       </c>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
@@ -1238,12 +1251,16 @@
       <c r="E21" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="2"/>
+    </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
         <v>50</v>
       </c>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1577,6 +1594,137 @@
         <v>1</v>
       </c>
     </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="7">
+        <v>1</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="23" t="str">
+        <f>"new RelacionTecnicoRol {TecnicoId = " &amp; B42 &amp; ", RolId = " &amp; D42 &amp; "},"</f>
+        <v>new RelacionTecnicoRol {TecnicoId = 57bf6b3f-26f0-4eaa-9f66-14b3e6fdfce2, RolId = Operador de Cabina 03 y Estudio de Radio},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="7">
+        <v>2</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43" s="23" t="str">
+        <f t="shared" ref="F43:F49" si="0">"new RelacionTecnicoRol {TecnicoId = " &amp; B43 &amp; ", RolId = " &amp; D43 &amp; "},"</f>
+        <v>new RelacionTecnicoRol {TecnicoId = 57bf6b3f-26f0-4eaa-9f66-14b3e6fdfce2, RolId = Sonidista},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="7">
+        <v>3</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>new RelacionTecnicoRol {TecnicoId = 0626bd2e-c394-4f89-bb52-8dcf01b0128c, RolId = Presentador / conductor},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="7">
+        <v>4</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>new RelacionTecnicoRol {TecnicoId = 0626bd2e-c394-4f89-bb52-8dcf01b0128c, RolId = Sonidista},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="7">
+        <v>5</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>new RelacionTecnicoRol {TecnicoId = 0626bd2e-c394-4f89-bb52-8dcf01b0128c, RolId = Redactor creativo},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="7">
+        <v>6</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>new RelacionTecnicoRol {TecnicoId = cf374546-893e-4b69-8622-a334fb02ade8, RolId = Operador de Cabina 02},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="7">
+        <v>7</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F48" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>new RelacionTecnicoRol {TecnicoId = cf374546-893e-4b69-8622-a334fb02ade8, RolId = Diseñador gráfico},</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="7">
+        <v>8</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F49" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>new RelacionTecnicoRol {TecnicoId = cf374546-893e-4b69-8622-a334fb02ade8, RolId = Cámara y asistente de cámara},</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>